<commit_message>
xls data table, variable sheet corrected
</commit_message>
<xml_diff>
--- a/Data_Analysis1/TeamAssignment_Eszter_Ozan_Viki/Restaurant_Research_DA1.xlsx
+++ b/Data_Analysis1/TeamAssignment_Eszter_Ozan_Viki/Restaurant_Research_DA1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diama\Documents\CEU-Business-Analytics-2020\Data_Analysis1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diama\Documents\CEU-Business-Analytics-2020\Data_Analysis1\TeamAssignment_Eszter_Ozan_Viki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD67A20-07A2-4E06-9384-E39D1301D2F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B64704-7295-4D09-98CE-639BE3212989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Restaurants" sheetId="2" r:id="rId1"/>
@@ -841,9 +841,6 @@
     <t>delivery_ceu</t>
   </si>
   <si>
-    <t>The medium of delviery, if the restaurant delivers to CEU</t>
-  </si>
-  <si>
     <t>delivery_medium</t>
   </si>
   <si>
@@ -898,10 +895,13 @@
     <t>pepsi_price</t>
   </si>
   <si>
-    <t>Margarita price alone</t>
-  </si>
-  <si>
     <t>margarita_price_alone</t>
+  </si>
+  <si>
+    <t>The medium of delviery</t>
+  </si>
+  <si>
+    <t>Price ti eat a margarita pizza (including delivery costs if applicable)</t>
   </si>
 </sst>
 </file>
@@ -9000,7 +9000,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection sqref="A1:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9411,10 +9411,10 @@
         <v>220</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>269</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -9425,10 +9425,10 @@
         <v>220</v>
       </c>
       <c r="C30" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -9442,7 +9442,7 @@
         <v>26</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -9453,10 +9453,10 @@
         <v>236</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>274</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -9467,10 +9467,10 @@
         <v>236</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -9481,10 +9481,10 @@
         <v>236</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -9495,10 +9495,10 @@
         <v>236</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -9509,10 +9509,10 @@
         <v>236</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>282</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -9523,10 +9523,10 @@
         <v>236</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -9537,10 +9537,10 @@
         <v>236</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -9551,10 +9551,10 @@
         <v>236</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>